<commit_message>
Introdotti dei difetti nei dati
</commit_message>
<xml_diff>
--- a/lez_19_20/lez_2x2/data.xlsx
+++ b/lez_19_20/lez_2x2/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Giovanni/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Giovanni/Dottorato/R Projects/CorsoStatisticaR/lez_19_20/lez_2x2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Pseudotsuga menziesii</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Plot_28</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -547,7 +553,7 @@
   <dimension ref="A1:AE29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,8 +851,8 @@
       <c r="C4" s="4">
         <v>0</v>
       </c>
-      <c r="D4" s="4">
-        <v>0</v>
+      <c r="D4" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
@@ -940,8 +946,8 @@
       <c r="C5" s="4">
         <v>37.5</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
+      <c r="D5" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
@@ -1035,8 +1041,8 @@
       <c r="C6" s="4">
         <v>3</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
+      <c r="D6" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
@@ -1130,9 +1136,7 @@
       <c r="C7" s="4">
         <v>3</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4">
         <v>0</v>
       </c>
@@ -1225,9 +1229,7 @@
       <c r="C8" s="4">
         <v>3</v>
       </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="4">
         <v>0</v>
       </c>
@@ -1320,9 +1322,7 @@
       <c r="C9" s="4">
         <v>0</v>
       </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="4">
         <v>0</v>
       </c>

</xml_diff>